<commit_message>
EPBDS-6931 Add test for concatenate() function
--HG--
branch : 5.19.x
</commit_message>
<xml_diff>
--- a/DEV/org.openl.test/test-resources/functionality/String.xlsx
+++ b/DEV/org.openl.test/test-resources/functionality/String.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="225" windowWidth="16140" windowHeight="9090" tabRatio="711"/>
+    <workbookView xWindow="285" yWindow="225" windowWidth="16140" windowHeight="9090" tabRatio="711" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="contains" sheetId="5" r:id="rId1"/>
@@ -14,13 +14,14 @@
     <sheet name="remove" sheetId="13" r:id="rId5"/>
     <sheet name="replace" sheetId="14" r:id="rId6"/>
     <sheet name="substring" sheetId="17" r:id="rId7"/>
+    <sheet name="concatenate" sheetId="18" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="225">
   <si>
     <t>return contains(str, searchChar);</t>
   </si>
@@ -626,6 +627,75 @@
   </si>
   <si>
     <t>,,,</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>=concatenate($C)</t>
+  </si>
+  <si>
+    <t>=concatenate($D)</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>=concatenate($D, 5)</t>
+  </si>
+  <si>
+    <t>=concatenate("S", 5)</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>=concatenate("S", '/', null, $D, 5, 3.1)</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult concatenate()</t>
+  </si>
+  <si>
+    <t>=concatenate("Hello")</t>
+  </si>
+  <si>
+    <t>Test concatenate concatenateTest()</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>S/1.553.1</t>
+  </si>
+  <si>
+    <t>1.55</t>
   </si>
 </sst>
 </file>
@@ -866,7 +936,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -919,8 +989,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -940,8 +1011,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1307,7 +1384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
@@ -1320,29 +1397,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
+      <c r="B3" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="54"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -1581,25 +1658,25 @@
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="54" t="s">
+      <c r="B34" s="55" t="s">
         <v>167</v>
       </c>
-      <c r="C34" s="54"/>
-      <c r="D34" s="54"/>
+      <c r="C34" s="55"/>
+      <c r="D34" s="55"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="56" t="s">
+      <c r="B35" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="56"/>
-      <c r="D35" s="56"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="51" t="s">
+      <c r="B37" s="52" t="s">
         <v>168</v>
       </c>
-      <c r="C37" s="52"/>
-      <c r="D37" s="53"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="54"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
@@ -1767,7 +1844,7 @@
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B53" s="25">
         <f ca="1">TODAY()</f>
-        <v>42271</v>
+        <v>43019</v>
       </c>
       <c r="C53" s="19" t="s">
         <v>181</v>
@@ -1872,25 +1949,25 @@
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B69" s="54" t="s">
+      <c r="B69" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="C69" s="55"/>
-      <c r="D69" s="55"/>
+      <c r="C69" s="56"/>
+      <c r="D69" s="56"/>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B70" s="56" t="s">
+      <c r="B70" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C70" s="56"/>
-      <c r="D70" s="56"/>
+      <c r="C70" s="57"/>
+      <c r="D70" s="57"/>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B72" s="51" t="s">
+      <c r="B72" s="52" t="s">
         <v>170</v>
       </c>
-      <c r="C72" s="52"/>
-      <c r="D72" s="53"/>
+      <c r="C72" s="53"/>
+      <c r="D72" s="54"/>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B73" s="5" t="s">
@@ -2107,25 +2184,25 @@
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B99" s="54" t="s">
+      <c r="B99" s="55" t="s">
         <v>171</v>
       </c>
-      <c r="C99" s="54"/>
-      <c r="D99" s="54"/>
+      <c r="C99" s="55"/>
+      <c r="D99" s="55"/>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B100" s="50" t="s">
+      <c r="B100" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="C100" s="50"/>
-      <c r="D100" s="50"/>
+      <c r="C100" s="58"/>
+      <c r="D100" s="58"/>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B102" s="51" t="s">
+      <c r="B102" s="52" t="s">
         <v>172</v>
       </c>
-      <c r="C102" s="52"/>
-      <c r="D102" s="53"/>
+      <c r="C102" s="53"/>
+      <c r="D102" s="54"/>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B103" s="5" t="s">
@@ -2354,11 +2431,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
     <mergeCell ref="B100:D100"/>
     <mergeCell ref="B102:D102"/>
     <mergeCell ref="B37:D37"/>
@@ -2366,6 +2438,11 @@
     <mergeCell ref="B70:D70"/>
     <mergeCell ref="B72:D72"/>
     <mergeCell ref="B99:D99"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2389,25 +2466,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="54"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -2646,25 +2723,25 @@
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="54" t="s">
+      <c r="B32" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="C32" s="54"/>
-      <c r="D32" s="54"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="50" t="s">
+      <c r="B33" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="C33" s="50"/>
-      <c r="D33" s="50"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="58"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="51" t="s">
+      <c r="B35" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="C35" s="52"/>
-      <c r="D35" s="53"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="54"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
@@ -2826,22 +2903,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="54"/>
+      <c r="C2" s="55"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="50"/>
+      <c r="C3" s="58"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="57"/>
+      <c r="C5" s="59"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="41" t="s">
@@ -2940,7 +3017,7 @@
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="25">
         <f ca="1">TODAY()</f>
-        <v>42271</v>
+        <v>43019</v>
       </c>
       <c r="C18" s="18" t="b">
         <v>0</v>
@@ -2988,22 +3065,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="54"/>
+      <c r="C2" s="55"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="50"/>
+      <c r="C3" s="58"/>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="57"/>
+      <c r="C5" s="59"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -3062,22 +3139,22 @@
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="54" t="s">
+      <c r="B18" s="55" t="s">
         <v>159</v>
       </c>
-      <c r="C18" s="54"/>
+      <c r="C18" s="55"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="58" t="s">
         <v>160</v>
       </c>
-      <c r="C19" s="50"/>
+      <c r="C19" s="58"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="57" t="s">
+      <c r="B21" s="59" t="s">
         <v>161</v>
       </c>
-      <c r="C21" s="57"/>
+      <c r="C21" s="59"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
@@ -3165,25 +3242,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="54"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -3334,25 +3411,25 @@
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="50" t="s">
+      <c r="B27" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="58"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="51" t="s">
+      <c r="B29" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="52"/>
-      <c r="D29" s="53"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="54"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
@@ -3484,7 +3561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -3498,28 +3575,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="54"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -3751,31 +3828,31 @@
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="55" t="s">
         <v>173</v>
       </c>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="54"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B30" s="50" t="s">
+      <c r="B30" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B32" s="51" t="s">
+      <c r="B32" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="C32" s="52"/>
-      <c r="D32" s="52"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="54"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
@@ -3960,25 +4037,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="52" t="s">
         <v>135</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="54"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
@@ -4067,28 +4144,28 @@
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="55" t="s">
         <v>136</v>
       </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="50" t="s">
+      <c r="B20" s="58" t="s">
         <v>132</v>
       </c>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="52" t="s">
         <v>137</v>
       </c>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="53"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="54"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="41" t="s">
@@ -4213,4 +4290,191 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="60" t="s">
+        <v>217</v>
+      </c>
+      <c r="C3" s="60"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F4" s="60" t="s">
+        <v>219</v>
+      </c>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>218</v>
+      </c>
+      <c r="F5" t="str">
+        <f>"_res_.$Formula$"&amp;B5</f>
+        <v>_res_.$Formula$A</v>
+      </c>
+      <c r="G5" t="str">
+        <f>B5</f>
+        <v>A</v>
+      </c>
+      <c r="H5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ref="F6:F12" si="0">"_res_.$Formula$"&amp;B6</f>
+        <v>_res_.$Formula$B</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" ref="G6:G12" si="1">B6</f>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>206</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>_res_.$Formula$C</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C8" s="51">
+        <v>1.5</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>_res_.$Formula$D</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v>D</v>
+      </c>
+      <c r="H8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>210</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>_res_.$Formula$E</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v>E</v>
+      </c>
+      <c r="H9" s="50" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>213</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>_res_.$Formula$F</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+      <c r="H10" s="50" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>212</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>214</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>_res_.$Formula$G</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v>G</v>
+      </c>
+      <c r="H11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>215</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>_res_.$Formula$H</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v>H</v>
+      </c>
+      <c r="H12" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>